<commit_message>
Update lexical diversity to output combined analysis file
</commit_message>
<xml_diff>
--- a/output/press_release/lexical_density_press_release.xlsx
+++ b/output/press_release/lexical_density_press_release.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="158">
   <si>
     <t>id</t>
   </si>
@@ -38,6 +38,9 @@
     <t>lexical_density</t>
   </si>
   <si>
+    <t>year</t>
+  </si>
+  <si>
     <t>http://www.politifact.com/truth-o-meter/statements/2009/apr/01/michele-bachmann/defending-dollar-bachmann-distorts-geithners-comme/</t>
   </si>
   <si>
@@ -501,9 +504,6 @@
   </si>
   <si>
     <t>max</t>
-  </si>
-  <si>
-    <t>year</t>
   </si>
 </sst>
 </file>
@@ -874,58 +874,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0.5568627450980392</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>0.5392405063291139</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>0.5436123348017621</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0.5751295336787565</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0.598404255319149</v>
+      </c>
+      <c r="C6">
+        <v>2009</v>
       </c>
     </row>
   </sheetData>
@@ -942,74 +960,98 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B2">
         <v>0.5369774919614148</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B3">
         <v>0.5976331360946746</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B4">
         <v>0.5902777777777778</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>0.6528189910979229</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B6">
         <v>0.625</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>0.6106870229007634</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B8">
         <v>0.5735294117647058</v>
+      </c>
+      <c r="C8">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>
@@ -1028,50 +1070,65 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2">
         <v>0.5833333333333334</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>0.5107398568019093</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B4">
         <v>0.555045871559633</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>0.5818033455732354</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -1081,74 +1138,98 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2">
         <v>0.6496350364963503</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>0.5366568914956011</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>0.6271929824561403</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>0.625</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>0.5308641975308642</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7">
         <v>0.5644067796610169</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B8">
         <v>0.6055555555555555</v>
+      </c>
+      <c r="C8">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -1158,98 +1239,131 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B2">
         <v>0.5436893203883495</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B3">
         <v>0.589041095890411</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>0.5705128205128205</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5">
         <v>0.559322033898305</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>0.6320166320166321</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B7">
         <v>0.5454545454545454</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B8">
         <v>0.5390070921985816</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B9">
         <v>0.6151832460732984</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B10">
         <v>0.5789473684210527</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B11">
         <v>0.5857142857142857</v>
+      </c>
+      <c r="C11">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -1259,66 +1373,87 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B2">
         <v>0.5955882352941176</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B3">
         <v>0.5277337559429477</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B4">
         <v>0.5365853658536586</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B5">
         <v>0.6024464831804281</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>0.5643115942028986</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <v>0.5587734241908007</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
       </c>
     </row>
   </sheetData>
@@ -1328,26 +1463,32 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B2">
         <v>0.565597667638484</v>
+      </c>
+      <c r="C2">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>
@@ -1357,42 +1498,54 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B2">
         <v>0.6065573770491803</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B3">
         <v>0.5759717314487632</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B4">
         <v>0.5602409638554217</v>
+      </c>
+      <c r="C4">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>
@@ -1410,31 +1563,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1905,82 +2058,109 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0.5891891891891892</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0.6348314606741573</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0.6352040816326531</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0.5494505494505495</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0.6336633663366337</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>0.6065573770491803</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>0.5729166666666666</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>0.5892857142857143</v>
+      </c>
+      <c r="C9">
+        <v>2010</v>
       </c>
     </row>
   </sheetData>
@@ -2000,154 +2180,208 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>0.6310975609756098</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>0.531496062992126</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>0.5272727272727272</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>0.6135593220338983</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>0.5847750865051903</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>0.5337519623233909</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>0.5986696230598669</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>0.5577395577395577</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>0.5295857988165681</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>0.5764705882352941</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>0.581888246628131</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>0.6043557168784029</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>0.548689138576779</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>0.5752212389380531</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>0.6037735849056604</v>
+      </c>
+      <c r="C18">
+        <v>2011</v>
       </c>
     </row>
   </sheetData>
@@ -2176,114 +2410,153 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>0.609375</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>0.4986945169712794</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>0.5831533477321814</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>0.5933429811866859</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>0.593939393939394</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>0.5720524017467249</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>0.6037735849056604</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>0.6050632911392405</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>0.5530546623794212</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>0.5888888888888889</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>0.5609756097560976</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>0.5082872928176796</v>
+      </c>
+      <c r="C13">
+        <v>2012</v>
       </c>
     </row>
   </sheetData>
@@ -2307,154 +2580,208 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>0.589622641509434</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>0.6104417670682731</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>0.5706293706293706</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>0.6551724137931034</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.6090909090909091</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>0.6291390728476821</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.6008583690987125</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>0.6060606060606061</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>0.5979381443298969</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>0.638095238095238</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>0.574468085106383</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13">
         <v>0.5376344086021505</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14">
         <v>0.6180257510729614</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>0.5779220779220779</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>0.553921568627451</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <v>0.5557432432432432</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B18">
         <v>0.4666666666666667</v>
+      </c>
+      <c r="C18">
+        <v>2013</v>
       </c>
     </row>
   </sheetData>
@@ -2483,106 +2810,142 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>0.5645756457564576</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>0.5854978354978355</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>0.5747126436781609</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>0.5833333333333334</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>0.5636363636363636</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7">
         <v>0.6461538461538462</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>0.5953757225433526</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B9">
         <v>0.625</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>0.5662285136501517</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B11">
         <v>0.5420289855072464</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B12">
         <v>0.5854978354978355</v>
+      </c>
+      <c r="C12">
+        <v>2014</v>
       </c>
     </row>
   </sheetData>
@@ -2605,74 +2968,98 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <v>0.637123745819398</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>0.5115384615384615</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>0.5911111111111111</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>0.5671981776765376</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>0.6018376722817764</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B7">
         <v>0.5341365461847389</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8">
         <v>0.5721925133689839</v>
+      </c>
+      <c r="C8">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>
@@ -2691,130 +3078,175 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2">
         <v>0.6382978723404256</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3">
         <v>0.6043956043956044</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>0.5852272727272727</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5">
         <v>0.6133333333333333</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B6">
         <v>0.6169590643274854</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B7">
         <v>0.6796875</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B8">
         <v>0.5642201834862385</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B9">
         <v>0.5632183908045977</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B10">
         <v>0.5685071574642127</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B11">
         <v>0.6190476190476191</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B12">
         <v>0.5340314136125655</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B13">
         <v>0.6226415094339622</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B14">
         <v>0.5714285714285714</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B15">
         <v>0.5738095238095238</v>
+      </c>
+      <c r="C15">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>
@@ -2840,162 +3272,219 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>0.5778748180494906</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B3">
         <v>0.6455026455026455</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B4">
         <v>0.5737211634904714</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B5">
         <v>0.5774647887323944</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B6">
         <v>0.5792682926829268</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B7">
         <v>0.638235294117647</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B8">
         <v>0.5791505791505791</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B9">
         <v>0.5522598870056498</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B10">
         <v>0.5603985056039851</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B11">
         <v>0.5560816809707014</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B12">
         <v>0.6289592760180995</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>0.6713286713286714</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B14">
         <v>0.5574425574425574</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B15">
         <v>0.5483870967741935</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B16">
         <v>0.6060100166944908</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B17">
         <v>0.5362840967575914</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B18">
         <v>0.6759776536312849</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B19">
         <v>0.5225225225225225</v>
+      </c>
+      <c r="C19">
+        <v>2017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>